<commit_message>
update the values from the ellipsoid brochure
</commit_message>
<xml_diff>
--- a/docs/Ellipsoid_Brochure_Info.xlsx
+++ b/docs/Ellipsoid_Brochure_Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\segmentation-eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFDA04A-428A-4D57-949D-123A3230D6BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69229FF-51F9-4A3F-A127-D778243CB202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="72">
   <si>
     <t>Device_name</t>
   </si>
@@ -58,10 +58,7 @@
     <t>least_axis_ablation_brochure</t>
   </si>
   <si>
-    <t>Energy_brochure</t>
-  </si>
-  <si>
-    <t>Predicted Ablation Volume (ml)</t>
+    <t>Energy_brochure(kJ)</t>
   </si>
   <si>
     <t>Covidien (Covidien MWA)</t>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>27.5 22.5 22.5</t>
+  </si>
+  <si>
+    <t>Predicted_Ablation_Volume</t>
   </si>
 </sst>
 </file>
@@ -598,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -647,21 +647,21 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>45</v>
@@ -670,13 +670,13 @@
         <v>150</v>
       </c>
       <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2">
         <v>12</v>
@@ -696,16 +696,16 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>45</v>
@@ -714,13 +714,13 @@
         <v>240</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3">
         <v>13</v>
@@ -740,16 +740,16 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>45</v>
@@ -758,13 +758,13 @@
         <v>300</v>
       </c>
       <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4">
         <v>13.5</v>
@@ -784,16 +784,16 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <v>45</v>
@@ -802,13 +802,13 @@
         <v>420</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5">
         <v>14</v>
@@ -828,16 +828,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>45</v>
@@ -846,13 +846,13 @@
         <v>600</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6">
         <v>14.5</v>
@@ -872,16 +872,16 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <v>75</v>
@@ -890,13 +890,13 @@
         <v>150</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7">
         <v>15</v>
@@ -916,16 +916,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8">
         <v>75</v>
@@ -934,13 +934,13 @@
         <v>240</v>
       </c>
       <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
         <v>25</v>
       </c>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J8">
         <v>16</v>
@@ -960,16 +960,16 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <v>75</v>
@@ -978,13 +978,13 @@
         <v>300</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9">
         <v>16.5</v>
@@ -1004,16 +1004,16 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10">
         <v>75</v>
@@ -1022,13 +1022,13 @@
         <v>420</v>
       </c>
       <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
         <v>28</v>
       </c>
-      <c r="H10" t="s">
-        <v>29</v>
-      </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J10">
         <v>17.5</v>
@@ -1048,16 +1048,16 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11">
         <v>75</v>
@@ -1066,13 +1066,13 @@
         <v>600</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11">
         <v>18</v>
@@ -1092,16 +1092,16 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -1110,13 +1110,13 @@
         <v>150</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J12">
         <v>17.5</v>
@@ -1136,16 +1136,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -1154,13 +1154,13 @@
         <v>240</v>
       </c>
       <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" t="s">
         <v>32</v>
       </c>
-      <c r="H13" t="s">
-        <v>33</v>
-      </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J13">
         <v>19</v>
@@ -1180,16 +1180,16 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -1198,13 +1198,13 @@
         <v>300</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J14">
         <v>19.5</v>
@@ -1224,16 +1224,16 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -1242,13 +1242,13 @@
         <v>420</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J15">
         <v>20</v>
@@ -1268,16 +1268,16 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -1286,13 +1286,13 @@
         <v>600</v>
       </c>
       <c r="G16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" t="s">
         <v>36</v>
       </c>
-      <c r="H16" t="s">
-        <v>37</v>
-      </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16">
         <v>20.5</v>
@@ -1312,16 +1312,16 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17">
         <v>20</v>
@@ -1330,13 +1330,13 @@
         <v>180</v>
       </c>
       <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="s">
         <v>40</v>
       </c>
-      <c r="H17" t="s">
-        <v>41</v>
-      </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J17">
         <v>12</v>
@@ -1356,16 +1356,16 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
         <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -1374,13 +1374,13 @@
         <v>300</v>
       </c>
       <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
         <v>42</v>
       </c>
-      <c r="H18" t="s">
-        <v>43</v>
-      </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J18">
         <v>13.5</v>
@@ -1400,16 +1400,16 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19">
         <v>20</v>
@@ -1418,13 +1418,13 @@
         <v>600</v>
       </c>
       <c r="G19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J19">
         <v>15.5</v>
@@ -1444,793 +1444,969 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
       <c r="C20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F20">
-        <v>180</v>
+        <v>900</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20">
+        <v>19</v>
+      </c>
+      <c r="K20">
+        <v>16.5</v>
+      </c>
+      <c r="L20">
+        <v>16.5</v>
+      </c>
+      <c r="M20">
         <v>18</v>
       </c>
-      <c r="J20">
-        <v>14.5</v>
-      </c>
-      <c r="K20">
-        <v>10</v>
-      </c>
-      <c r="L20">
-        <v>10</v>
-      </c>
-      <c r="M20">
-        <v>7.2</v>
-      </c>
       <c r="N20">
-        <v>6.0736999999999997</v>
+        <v>21.6676</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
       <c r="C21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <v>40</v>
       </c>
       <c r="F21">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="G21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H21" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J21">
-        <v>18</v>
+        <v>14.5</v>
       </c>
       <c r="K21">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="L21">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M21">
-        <v>12</v>
+        <v>7.2</v>
       </c>
       <c r="N21">
-        <v>14.7781</v>
+        <v>6.0736999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
       <c r="C22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22">
         <v>40</v>
       </c>
       <c r="F22">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22">
         <v>18</v>
       </c>
-      <c r="J22">
-        <v>24.5</v>
-      </c>
       <c r="K22">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L22">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M22">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="N22">
-        <v>33.250599999999999</v>
+        <v>14.7781</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
         <v>38</v>
       </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
       <c r="C23">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F23">
-        <v>180</v>
+        <v>600</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23">
+        <v>24.5</v>
+      </c>
+      <c r="K23">
         <v>18</v>
       </c>
-      <c r="J23">
-        <v>18.5</v>
-      </c>
-      <c r="K23">
-        <v>12.5</v>
-      </c>
       <c r="L23">
-        <v>12.5</v>
+        <v>18</v>
       </c>
       <c r="M23">
-        <v>10.8</v>
+        <v>24</v>
       </c>
       <c r="N23">
-        <v>12.1082</v>
+        <v>33.250599999999999</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
         <v>38</v>
       </c>
-      <c r="B24" t="s">
-        <v>39</v>
-      </c>
       <c r="C24">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F24">
-        <v>300</v>
+        <v>900</v>
       </c>
       <c r="G24" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K24">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="L24">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="M24">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="N24">
-        <v>29.0534</v>
+        <v>46.181399999999996</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
       <c r="C25">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25">
         <v>60</v>
       </c>
       <c r="F25">
-        <v>600</v>
+        <v>180</v>
       </c>
       <c r="G25" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J25">
-        <v>27</v>
+        <v>18.5</v>
       </c>
       <c r="K25">
-        <v>20</v>
+        <v>12.5</v>
       </c>
       <c r="L25">
-        <v>20</v>
+        <v>12.5</v>
       </c>
       <c r="M25">
-        <v>36</v>
+        <v>10.8</v>
       </c>
       <c r="N25">
-        <v>45.238900000000001</v>
+        <v>12.1082</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
         <v>38</v>
       </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
       <c r="C26">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E26">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F26">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="G26" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26">
+        <v>24</v>
+      </c>
+      <c r="K26">
+        <v>17</v>
+      </c>
+      <c r="L26">
+        <v>17</v>
+      </c>
+      <c r="M26">
         <v>18</v>
       </c>
-      <c r="J26">
-        <v>23</v>
-      </c>
-      <c r="K26">
-        <v>16</v>
-      </c>
-      <c r="L26">
-        <v>16</v>
-      </c>
-      <c r="M26">
-        <v>14.4</v>
-      </c>
       <c r="N26">
-        <v>24.663599999999999</v>
+        <v>29.0534</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
         <v>38</v>
       </c>
-      <c r="B27" t="s">
-        <v>39</v>
-      </c>
       <c r="C27">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E27">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F27">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="G27" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H27" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J27">
-        <v>25.5</v>
+        <v>27</v>
       </c>
       <c r="K27">
-        <v>18.5</v>
+        <v>20</v>
       </c>
       <c r="L27">
-        <v>18.5</v>
+        <v>20</v>
       </c>
       <c r="M27">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="N27">
-        <v>36.557099999999998</v>
+        <v>45.238900000000001</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s">
-        <v>39</v>
-      </c>
       <c r="C28">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E28">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F28">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="G28" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H28" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="I28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J28">
-        <v>33</v>
+        <v>30.5</v>
       </c>
       <c r="K28">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L28">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M28">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="N28">
-        <v>73.123699999999999</v>
+        <v>73.588700000000003</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F29">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="G29" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="I29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J29">
-        <v>13.5</v>
+        <v>23</v>
       </c>
       <c r="K29">
-        <v>11.5</v>
+        <v>16</v>
       </c>
       <c r="L29">
-        <v>11.5</v>
+        <v>16</v>
       </c>
       <c r="M29">
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
       <c r="N29">
-        <v>7.4786000000000001</v>
+        <v>24.663599999999999</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F30">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="G30" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H30" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J30">
+        <v>25.5</v>
+      </c>
+      <c r="K30">
         <v>18.5</v>
       </c>
-      <c r="K30">
-        <v>16.5</v>
-      </c>
       <c r="L30">
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
       <c r="M30">
-        <v>14.4</v>
+        <v>24</v>
       </c>
       <c r="N30">
-        <v>21.0974</v>
+        <v>36.557099999999998</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31">
+        <v>80</v>
+      </c>
+      <c r="F31">
+        <v>600</v>
+      </c>
+      <c r="G31" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31" t="s">
         <v>60</v>
       </c>
-      <c r="F31">
-        <v>360</v>
-      </c>
-      <c r="G31" t="s">
-        <v>35</v>
-      </c>
-      <c r="H31" t="s">
-        <v>65</v>
-      </c>
       <c r="I31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J31">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="K31">
-        <v>17.5</v>
+        <v>23</v>
       </c>
       <c r="L31">
-        <v>17.5</v>
+        <v>23</v>
       </c>
       <c r="M31">
-        <v>21.6</v>
+        <v>48</v>
       </c>
       <c r="N31">
-        <v>25.656300000000002</v>
+        <v>73.123699999999999</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F32">
-        <v>120</v>
+        <v>900</v>
       </c>
       <c r="G32" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H32" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J32">
-        <v>16</v>
+        <v>36.5</v>
       </c>
       <c r="K32">
-        <v>13.5</v>
+        <v>27.5</v>
       </c>
       <c r="L32">
-        <v>13.5</v>
+        <v>27.5</v>
       </c>
       <c r="M32">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="N32">
-        <v>12.214499999999999</v>
+        <v>115.6237</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33">
+        <v>60</v>
+      </c>
+      <c r="F33">
+        <v>120</v>
+      </c>
+      <c r="G33" t="s">
         <v>63</v>
       </c>
-      <c r="C33">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33">
-        <v>100</v>
-      </c>
-      <c r="F33">
-        <v>240</v>
-      </c>
-      <c r="G33" t="s">
-        <v>36</v>
-      </c>
       <c r="H33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J33">
-        <v>20.5</v>
+        <v>13.5</v>
       </c>
       <c r="K33">
-        <v>18</v>
+        <v>11.5</v>
       </c>
       <c r="L33">
-        <v>18</v>
+        <v>11.5</v>
       </c>
       <c r="M33">
-        <v>24</v>
+        <v>7.2</v>
       </c>
       <c r="N33">
-        <v>27.821899999999999</v>
+        <v>7.4786000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
         <v>62</v>
       </c>
-      <c r="B34" t="s">
-        <v>63</v>
-      </c>
       <c r="C34">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E34">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F34">
-        <v>360</v>
+        <v>240</v>
       </c>
       <c r="G34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J34">
-        <v>23.5</v>
+        <v>18.5</v>
       </c>
       <c r="K34">
-        <v>20</v>
+        <v>16.5</v>
       </c>
       <c r="L34">
-        <v>20</v>
+        <v>16.5</v>
       </c>
       <c r="M34">
-        <v>36</v>
+        <v>14.4</v>
       </c>
       <c r="N34">
-        <v>39.374600000000001</v>
+        <v>21.0974</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
         <v>62</v>
       </c>
-      <c r="B35" t="s">
-        <v>63</v>
-      </c>
       <c r="C35">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="F35">
-        <v>120</v>
+        <v>360</v>
       </c>
       <c r="G35" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="H35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J35">
+        <v>20</v>
+      </c>
+      <c r="K35">
         <v>17.5</v>
       </c>
-      <c r="K35">
-        <v>14.5</v>
-      </c>
       <c r="L35">
-        <v>14.5</v>
+        <v>17.5</v>
       </c>
       <c r="M35">
-        <v>16.8</v>
+        <v>21.6</v>
       </c>
       <c r="N35">
-        <v>15.412100000000001</v>
+        <v>25.656300000000002</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
         <v>62</v>
       </c>
-      <c r="B36" t="s">
-        <v>63</v>
-      </c>
       <c r="C36">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="F36">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="G36" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J36">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="K36">
-        <v>20.5</v>
+        <v>13.5</v>
       </c>
       <c r="L36">
-        <v>20.5</v>
+        <v>13.5</v>
       </c>
       <c r="M36">
-        <v>33.6</v>
+        <v>12</v>
       </c>
       <c r="N36">
-        <v>45.768799999999999</v>
+        <v>12.214499999999999</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
         <v>62</v>
       </c>
-      <c r="B37" t="s">
-        <v>63</v>
-      </c>
       <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37">
+        <v>240</v>
+      </c>
+      <c r="G37" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" t="s">
+        <v>64</v>
+      </c>
+      <c r="I37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37">
+        <v>20.5</v>
+      </c>
+      <c r="K37">
+        <v>18</v>
+      </c>
+      <c r="L37">
+        <v>18</v>
+      </c>
+      <c r="M37">
+        <v>24</v>
+      </c>
+      <c r="N37">
+        <v>27.821899999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38">
+        <v>100</v>
+      </c>
+      <c r="F38">
+        <v>360</v>
+      </c>
+      <c r="G38" t="s">
+        <v>67</v>
+      </c>
+      <c r="H38" t="s">
+        <v>64</v>
+      </c>
+      <c r="I38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38">
+        <v>23.5</v>
+      </c>
+      <c r="K38">
+        <v>20</v>
+      </c>
+      <c r="L38">
+        <v>20</v>
+      </c>
+      <c r="M38">
+        <v>36</v>
+      </c>
+      <c r="N38">
+        <v>39.374600000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <v>140</v>
+      </c>
+      <c r="F39">
+        <v>120</v>
+      </c>
+      <c r="G39" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" t="s">
+        <v>64</v>
+      </c>
+      <c r="I39" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39">
+        <v>17.5</v>
+      </c>
+      <c r="K39">
+        <v>14.5</v>
+      </c>
+      <c r="L39">
+        <v>14.5</v>
+      </c>
+      <c r="M39">
+        <v>16.8</v>
+      </c>
+      <c r="N39">
+        <v>15.412100000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40">
+        <v>140</v>
+      </c>
+      <c r="F40">
+        <v>240</v>
+      </c>
+      <c r="G40" t="s">
+        <v>69</v>
+      </c>
+      <c r="H40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I40" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40">
+        <v>26</v>
+      </c>
+      <c r="K40">
+        <v>20.5</v>
+      </c>
+      <c r="L40">
+        <v>20.5</v>
+      </c>
+      <c r="M40">
+        <v>33.6</v>
+      </c>
+      <c r="N40">
+        <v>45.768799999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41">
         <v>11</v>
       </c>
-      <c r="D37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37">
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41">
         <v>140</v>
       </c>
-      <c r="F37">
+      <c r="F41">
         <v>360</v>
       </c>
-      <c r="G37" t="s">
-        <v>71</v>
-      </c>
-      <c r="H37" t="s">
-        <v>65</v>
-      </c>
-      <c r="I37" t="s">
-        <v>18</v>
-      </c>
-      <c r="J37">
+      <c r="G41" t="s">
+        <v>70</v>
+      </c>
+      <c r="H41" t="s">
+        <v>64</v>
+      </c>
+      <c r="I41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41">
         <v>27.5</v>
       </c>
-      <c r="K37">
+      <c r="K41">
         <v>22.5</v>
       </c>
-      <c r="L37">
+      <c r="L41">
         <v>22.5</v>
       </c>
-      <c r="M37">
+      <c r="M41">
         <v>50.4</v>
       </c>
-      <c r="N37">
+      <c r="N41">
         <v>58.315800000000003</v>
       </c>
     </row>

</xml_diff>